<commit_message>
added pilot 2 sheet
</commit_message>
<xml_diff>
--- a/analysis/praise-draw_data.xlsx
+++ b/analysis/praise-draw_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinkcupcakes123/Documents/GitHub/praise-draw/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3659ACC9-3050-054E-A99F-1DCE520D7F06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87208BCD-A61C-214A-88D8-DD7F073A400B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16500" xr2:uid="{7F85E784-ACEF-194A-84B2-6A49ADD88783}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{7F85E784-ACEF-194A-84B2-6A49ADD88783}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pilot 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pilot 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="170">
   <si>
     <t>count</t>
   </si>
@@ -903,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035477AC-CE20-344D-9C0D-66946B13C514}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2917,4 +2918,114 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FDC708-1639-6547-A64F-F806FC16AE1E}">
+  <dimension ref="A1:AE1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
coded half of the videos
</commit_message>
<xml_diff>
--- a/analysis/praise-draw_data.xlsx
+++ b/analysis/praise-draw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinkcupcakes123/Documents/GitHub/praise-draw/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87208BCD-A61C-214A-88D8-DD7F073A400B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD742316-68F6-414F-8664-9FB104D58D57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{7F85E784-ACEF-194A-84B2-6A49ADD88783}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="209">
   <si>
     <t>count</t>
   </si>
@@ -542,6 +542,123 @@
   </si>
   <si>
     <t xml:space="preserve">unclear but not scribbles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">redo button below screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">molly </t>
+  </si>
+  <si>
+    <t>drawing1_notes</t>
+  </si>
+  <si>
+    <t>drawing2_notes</t>
+  </si>
+  <si>
+    <t>PD_190712_01</t>
+  </si>
+  <si>
+    <t>bb236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">because it doesn’t have scribble scribble </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cuz I like yellow and red </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cuz I like red </t>
+  </si>
+  <si>
+    <t>PD_190712_02</t>
+  </si>
+  <si>
+    <t>ba896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">because this one [points to bad one] is just a scribble scrabble </t>
+  </si>
+  <si>
+    <t>well kind of other kind of a little of the points from my flower kind of it was a little low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kind of because she was the one who I worked hardest for because the other time wait I did better points kind of I was trying to do that for the other teacher but I kind of got messed up a little </t>
+  </si>
+  <si>
+    <t>PD_190712_03</t>
+  </si>
+  <si>
+    <t>bb249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good </t>
+  </si>
+  <si>
+    <t xml:space="preserve">because it's not messy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">redo button below screen; drew a really long time for both, I didn’t have a protocol for time warnings yet  </t>
+  </si>
+  <si>
+    <t>can't see</t>
+  </si>
+  <si>
+    <t xml:space="preserve">both </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I don’t know </t>
+  </si>
+  <si>
+    <t>PD_190712_04</t>
+  </si>
+  <si>
+    <t>bb230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">because this one [good one] has a circle and this one [bad one] has a scribble scrabble </t>
+  </si>
+  <si>
+    <t>cuz I liked it a lot</t>
+  </si>
+  <si>
+    <t>because I like her t shirt</t>
+  </si>
+  <si>
+    <t>PD2_190715_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">because it looks like a flower that [bad one] is scribbling </t>
+  </si>
+  <si>
+    <t>bb226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don’t know </t>
+  </si>
+  <si>
+    <t>PD2_190715_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">because this one [bad] is only scribble scrabble and this one [good] is the right way </t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>**no</t>
+  </si>
+  <si>
+    <t>because</t>
+  </si>
+  <si>
+    <t xml:space="preserve">because  </t>
   </si>
 </sst>
 </file>
@@ -904,7 +1021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035477AC-CE20-344D-9C0D-66946B13C514}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection sqref="A1:AE1"/>
     </sheetView>
   </sheetViews>
@@ -2922,15 +3039,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FDC708-1639-6547-A64F-F806FC16AE1E}">
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+    <col min="14" max="14" width="16.5" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="18" customWidth="1"/>
+    <col min="18" max="18" width="16.1640625" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="20" width="18.33203125" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" customWidth="1"/>
+    <col min="22" max="22" width="19.1640625" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" customWidth="1"/>
+    <col min="26" max="26" width="23.5" customWidth="1"/>
+    <col min="27" max="27" width="12" customWidth="1"/>
+    <col min="28" max="28" width="22" customWidth="1"/>
+    <col min="29" max="29" width="24.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2998,31 +3145,579 @@
         <v>20</v>
       </c>
       <c r="W1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="X1" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="Y1" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="Z1" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="AA1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AB1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AC1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43658</v>
+      </c>
+      <c r="D2">
+        <v>4.67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" t="s">
+        <v>177</v>
+      </c>
+      <c r="M2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" t="s">
+        <v>178</v>
+      </c>
+      <c r="T2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" t="s">
+        <v>178</v>
+      </c>
+      <c r="W2" t="s">
+        <v>160</v>
+      </c>
+      <c r="X2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43658</v>
+      </c>
+      <c r="D3">
+        <v>5.31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="s">
+        <v>78</v>
+      </c>
+      <c r="P3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" t="s">
+        <v>92</v>
+      </c>
+      <c r="S3" t="s">
+        <v>178</v>
+      </c>
+      <c r="T3" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" t="s">
+        <v>92</v>
+      </c>
+      <c r="V3" t="s">
+        <v>178</v>
+      </c>
+      <c r="W3" t="s">
+        <v>160</v>
+      </c>
+      <c r="X3" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43658</v>
+      </c>
+      <c r="D4">
+        <v>4.08</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>187</v>
+      </c>
+      <c r="H4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>188</v>
+      </c>
+      <c r="L4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>75</v>
+      </c>
+      <c r="R4" t="s">
+        <v>92</v>
+      </c>
+      <c r="S4" t="s">
+        <v>178</v>
+      </c>
+      <c r="T4" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" t="s">
+        <v>92</v>
+      </c>
+      <c r="V4" t="s">
+        <v>178</v>
+      </c>
+      <c r="W4" t="s">
+        <v>160</v>
+      </c>
+      <c r="X4" t="s">
+        <v>191</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43658</v>
+      </c>
+      <c r="D5">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" t="s">
+        <v>171</v>
+      </c>
+      <c r="I5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
+        <v>188</v>
+      </c>
+      <c r="L5" t="s">
+        <v>196</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>75</v>
+      </c>
+      <c r="R5" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5" t="s">
+        <v>178</v>
+      </c>
+      <c r="T5" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" t="s">
+        <v>92</v>
+      </c>
+      <c r="V5" t="s">
+        <v>178</v>
+      </c>
+      <c r="W5" t="s">
+        <v>160</v>
+      </c>
+      <c r="X5" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43661</v>
+      </c>
+      <c r="D6">
+        <v>4.51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" t="s">
+        <v>200</v>
+      </c>
+      <c r="M6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R6" t="s">
+        <v>92</v>
+      </c>
+      <c r="S6" t="s">
+        <v>178</v>
+      </c>
+      <c r="T6" t="s">
+        <v>43</v>
+      </c>
+      <c r="U6" t="s">
+        <v>92</v>
+      </c>
+      <c r="V6" t="s">
+        <v>178</v>
+      </c>
+      <c r="W6" t="s">
+        <v>160</v>
+      </c>
+      <c r="X6" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43661</v>
+      </c>
+      <c r="D7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>205</v>
+      </c>
+      <c r="H7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" t="s">
+        <v>204</v>
+      </c>
+      <c r="M7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" t="s">
+        <v>78</v>
+      </c>
+      <c r="O7" t="s">
+        <v>73</v>
+      </c>
+      <c r="P7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7" t="s">
+        <v>92</v>
+      </c>
+      <c r="S7" t="s">
+        <v>178</v>
+      </c>
+      <c r="T7" t="s">
+        <v>43</v>
+      </c>
+      <c r="U7" t="s">
+        <v>92</v>
+      </c>
+      <c r="V7" t="s">
+        <v>178</v>
+      </c>
+      <c r="W7" t="s">
+        <v>191</v>
+      </c>
+      <c r="X7" t="s">
+        <v>191</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>171</v>
+      </c>
+      <c r="I11" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made new quality ratings tab
</commit_message>
<xml_diff>
--- a/analysis/praise-draw_data.xlsx
+++ b/analysis/praise-draw_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinkcupcakes123/Documents/GitHub/praise-draw/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD35ECA-B0F7-4C4B-9DD0-CC1E01179B99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A982455-9E50-9945-9036-4E15ED5A4B0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="680" windowWidth="28040" windowHeight="16500" activeTab="2" xr2:uid="{7F85E784-ACEF-194A-84B2-6A49ADD88783}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilot 1" sheetId="1" r:id="rId1"/>
     <sheet name="Pilot 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Pilot 2 - Alums" sheetId="3" r:id="rId3"/>
+    <sheet name="Quality Ratings" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="377">
   <si>
     <t>count</t>
   </si>
@@ -3545,11 +3545,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FDC708-1639-6547-A64F-F806FC16AE1E}">
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0">
+    <sheetView topLeftCell="V1" zoomScale="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6687,19 +6687,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>350</v>
+        <v>367</v>
       </c>
       <c r="C33" s="2">
         <v>43682</v>
       </c>
       <c r="D33">
-        <v>5.84</v>
+        <v>6.73</v>
       </c>
       <c r="E33" t="s">
         <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="G33" t="s">
         <v>40</v>
@@ -6714,7 +6714,7 @@
         <v>67</v>
       </c>
       <c r="K33" t="s">
-        <v>351</v>
+        <v>369</v>
       </c>
       <c r="L33" t="s">
         <v>43</v>
@@ -6726,7 +6726,7 @@
         <v>44</v>
       </c>
       <c r="O33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P33" t="s">
         <v>43</v>
@@ -6747,37 +6747,37 @@
         <v>68</v>
       </c>
       <c r="V33" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="W33" t="s">
         <v>142</v>
       </c>
       <c r="X33" t="s">
-        <v>342</v>
+        <v>68</v>
       </c>
       <c r="Y33" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="Z33" t="s">
-        <v>142</v>
+        <v>292</v>
       </c>
       <c r="AA33" t="s">
-        <v>342</v>
+        <v>68</v>
       </c>
       <c r="AB33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AC33" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
       <c r="AD33" t="s">
         <v>45</v>
       </c>
       <c r="AE33" t="s">
-        <v>355</v>
+        <v>371</v>
       </c>
       <c r="AF33" t="s">
-        <v>353</v>
+        <v>372</v>
       </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.2">
@@ -6785,7 +6785,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C34" s="2">
         <v>43682</v>
@@ -6797,7 +6797,7 @@
         <v>39</v>
       </c>
       <c r="F34" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="G34" t="s">
         <v>40</v>
@@ -6812,7 +6812,7 @@
         <v>67</v>
       </c>
       <c r="K34" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="L34" t="s">
         <v>43</v>
@@ -6827,13 +6827,13 @@
         <v>44</v>
       </c>
       <c r="P34" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="Q34" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="R34" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="S34" t="s">
         <v>43</v>
@@ -6848,7 +6848,7 @@
         <v>72</v>
       </c>
       <c r="W34" t="s">
-        <v>359</v>
+        <v>142</v>
       </c>
       <c r="X34" t="s">
         <v>342</v>
@@ -6857,7 +6857,7 @@
         <v>72</v>
       </c>
       <c r="Z34" t="s">
-        <v>287</v>
+        <v>142</v>
       </c>
       <c r="AA34" t="s">
         <v>342</v>
@@ -6866,13 +6866,16 @@
         <v>44</v>
       </c>
       <c r="AC34" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AD34" t="s">
         <v>45</v>
       </c>
       <c r="AE34" t="s">
-        <v>361</v>
+        <v>355</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.2">
@@ -6880,19 +6883,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C35" s="2">
         <v>43682</v>
       </c>
       <c r="D35">
-        <v>4.5599999999999996</v>
+        <v>5.84</v>
       </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="G35" t="s">
         <v>40</v>
@@ -6907,28 +6910,28 @@
         <v>67</v>
       </c>
       <c r="K35" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="L35" t="s">
         <v>43</v>
       </c>
       <c r="M35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P35" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="Q35" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="R35" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="S35" t="s">
         <v>43</v>
@@ -6943,10 +6946,10 @@
         <v>72</v>
       </c>
       <c r="W35" t="s">
-        <v>287</v>
+        <v>359</v>
       </c>
       <c r="X35" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="Y35" t="s">
         <v>72</v>
@@ -6958,16 +6961,206 @@
         <v>342</v>
       </c>
       <c r="AB35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AC35" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>362</v>
+      </c>
+      <c r="C36" s="2">
+        <v>43682</v>
+      </c>
+      <c r="D36">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="E36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" t="s">
+        <v>364</v>
+      </c>
+      <c r="G36" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" t="s">
+        <v>41</v>
+      </c>
+      <c r="I36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J36" t="s">
+        <v>67</v>
+      </c>
+      <c r="K36" t="s">
+        <v>363</v>
+      </c>
+      <c r="L36" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36" t="s">
+        <v>44</v>
+      </c>
+      <c r="N36" t="s">
+        <v>45</v>
+      </c>
+      <c r="O36" t="s">
+        <v>45</v>
+      </c>
+      <c r="P36" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>46</v>
+      </c>
+      <c r="R36" t="s">
+        <v>68</v>
+      </c>
+      <c r="S36" t="s">
+        <v>43</v>
+      </c>
+      <c r="T36" t="s">
+        <v>46</v>
+      </c>
+      <c r="U36" t="s">
+        <v>68</v>
+      </c>
+      <c r="V36" t="s">
+        <v>72</v>
+      </c>
+      <c r="W36" t="s">
+        <v>287</v>
+      </c>
+      <c r="X36" t="s">
+        <v>365</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>287</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC36" t="s">
         <v>366</v>
       </c>
-      <c r="AD35" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE35" t="s">
+      <c r="AD36" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE36" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>373</v>
+      </c>
+      <c r="C37" s="2">
+        <v>43683</v>
+      </c>
+      <c r="D37">
+        <v>6.51</v>
+      </c>
+      <c r="E37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" t="s">
+        <v>375</v>
+      </c>
+      <c r="G37" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" t="s">
+        <v>67</v>
+      </c>
+      <c r="K37" t="s">
+        <v>374</v>
+      </c>
+      <c r="L37" t="s">
+        <v>43</v>
+      </c>
+      <c r="M37" t="s">
+        <v>44</v>
+      </c>
+      <c r="N37" t="s">
+        <v>45</v>
+      </c>
+      <c r="O37" t="s">
+        <v>45</v>
+      </c>
+      <c r="P37" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>46</v>
+      </c>
+      <c r="R37" t="s">
+        <v>68</v>
+      </c>
+      <c r="S37" t="s">
+        <v>43</v>
+      </c>
+      <c r="T37" t="s">
+        <v>46</v>
+      </c>
+      <c r="U37" t="s">
+        <v>68</v>
+      </c>
+      <c r="V37" t="s">
+        <v>142</v>
+      </c>
+      <c r="W37" t="s">
+        <v>142</v>
+      </c>
+      <c r="X37" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>376</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -6976,336 +7169,425 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AA399A-D8CF-C643-ACB9-43959DA58862}">
-  <dimension ref="A1:AF3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCF0D24-0A3F-5B4C-B64B-3F8F6122393A}">
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" customWidth="1"/>
-    <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="18.5" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" customWidth="1"/>
-    <col min="18" max="18" width="19.33203125" customWidth="1"/>
-    <col min="19" max="19" width="18.33203125" customWidth="1"/>
-    <col min="20" max="20" width="16" customWidth="1"/>
-    <col min="21" max="21" width="19.1640625" customWidth="1"/>
-    <col min="22" max="22" width="15.6640625" customWidth="1"/>
-    <col min="23" max="23" width="14.5" customWidth="1"/>
-    <col min="24" max="24" width="19.83203125" customWidth="1"/>
-    <col min="25" max="25" width="15.6640625" customWidth="1"/>
-    <col min="26" max="26" width="14.1640625" customWidth="1"/>
-    <col min="27" max="27" width="20.33203125" customWidth="1"/>
-    <col min="28" max="28" width="13.1640625" customWidth="1"/>
-    <col min="29" max="29" width="23" customWidth="1"/>
-    <col min="30" max="30" width="12.33203125" customWidth="1"/>
-    <col min="31" max="31" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>240</v>
-      </c>
-      <c r="W1" t="s">
-        <v>173</v>
-      </c>
-      <c r="X1" t="s">
-        <v>339</v>
-      </c>
-      <c r="Y1" t="s">
         <v>241</v>
       </c>
-      <c r="Z1" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>340</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>175</v>
       </c>
       <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B16" t="s">
+        <v>243</v>
+      </c>
+      <c r="C16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" t="s">
+        <v>243</v>
+      </c>
+      <c r="C17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>270</v>
+      </c>
+      <c r="B19" t="s">
+        <v>267</v>
+      </c>
+      <c r="C19" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>276</v>
+      </c>
+      <c r="B20" t="s">
+        <v>280</v>
+      </c>
+      <c r="C20" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B21" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>295</v>
+      </c>
+      <c r="B23" t="s">
+        <v>280</v>
+      </c>
+      <c r="C23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>298</v>
+      </c>
+      <c r="B24" t="s">
+        <v>280</v>
+      </c>
+      <c r="C24" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>302</v>
+      </c>
+      <c r="B25" t="s">
+        <v>305</v>
+      </c>
+      <c r="C25" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>310</v>
+      </c>
+      <c r="B26" t="s">
+        <v>305</v>
+      </c>
+      <c r="C26" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>316</v>
+      </c>
+      <c r="B27" t="s">
+        <v>305</v>
+      </c>
+      <c r="C27" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>321</v>
+      </c>
+      <c r="B28" t="s">
+        <v>305</v>
+      </c>
+      <c r="C28" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>326</v>
+      </c>
+      <c r="B29" t="s">
+        <v>305</v>
+      </c>
+      <c r="C29" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>331</v>
+      </c>
+      <c r="B30" t="s">
+        <v>305</v>
+      </c>
+      <c r="C30" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>345</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>367</v>
       </c>
-      <c r="C2" s="2">
-        <v>43682</v>
-      </c>
-      <c r="D2">
-        <v>6.73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>368</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
-        <v>67</v>
-      </c>
-      <c r="K2" t="s">
-        <v>369</v>
-      </c>
-      <c r="L2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" t="s">
-        <v>68</v>
-      </c>
-      <c r="S2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" t="s">
-        <v>46</v>
-      </c>
-      <c r="U2" t="s">
-        <v>68</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="B33" t="s">
         <v>142</v>
       </c>
-      <c r="W2" t="s">
+      <c r="C33" t="s">
         <v>142</v>
       </c>
-      <c r="X2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y2" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>350</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>356</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>362</v>
+      </c>
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>373</v>
+      </c>
+      <c r="B37" t="s">
         <v>142</v>
       </c>
-      <c r="Z2" t="s">
-        <v>292</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>370</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>371</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>373</v>
-      </c>
-      <c r="C3" s="2">
-        <v>43683</v>
-      </c>
-      <c r="D3">
-        <v>6.51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>375</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" t="s">
-        <v>374</v>
-      </c>
-      <c r="L3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" t="s">
-        <v>68</v>
-      </c>
-      <c r="S3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" t="s">
-        <v>46</v>
-      </c>
-      <c r="U3" t="s">
-        <v>68</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="C37" t="s">
         <v>142</v>
-      </c>
-      <c r="W3" t="s">
-        <v>142</v>
-      </c>
-      <c r="X3" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>142</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>142</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>376</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made quality ratings tab
</commit_message>
<xml_diff>
--- a/analysis/praise-draw_data.xlsx
+++ b/analysis/praise-draw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinkcupcakes123/Documents/GitHub/praise-draw/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A982455-9E50-9945-9036-4E15ED5A4B0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C681C5ED-055E-1146-B85F-C9F05FD107A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="680" windowWidth="28040" windowHeight="16500" activeTab="2" xr2:uid="{7F85E784-ACEF-194A-84B2-6A49ADD88783}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="382">
   <si>
     <t>count</t>
   </si>
@@ -1164,6 +1164,21 @@
   </si>
   <si>
     <t>because I haven't been practicing on drawing that kind of flower</t>
+  </si>
+  <si>
+    <t>a flower</t>
+  </si>
+  <si>
+    <t>visual_cue</t>
+  </si>
+  <si>
+    <t>a flower garden</t>
+  </si>
+  <si>
+    <t>some flowers</t>
+  </si>
+  <si>
+    <t>a slice of watermelon</t>
   </si>
 </sst>
 </file>
@@ -3547,9 +3562,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FDC708-1639-6547-A64F-F806FC16AE1E}">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="109" workbookViewId="0">
+    <sheetView zoomScale="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y1" sqref="Y1:Y1048576"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7170,10 +7185,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCF0D24-0A3F-5B4C-B64B-3F8F6122393A}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7183,7 +7198,7 @@
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7193,327 +7208,417 @@
       <c r="C1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>186</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>201</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>206</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>212</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>215</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>221</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>226</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>237</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>379</v>
       </c>
       <c r="C14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>245</v>
       </c>
       <c r="B15" t="s">
-        <v>243</v>
+        <v>379</v>
       </c>
       <c r="C15" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>251</v>
       </c>
       <c r="B16" t="s">
-        <v>243</v>
+        <v>379</v>
       </c>
       <c r="C16" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>257</v>
       </c>
       <c r="B17" t="s">
-        <v>243</v>
+        <v>379</v>
       </c>
       <c r="C17" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>263</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>379</v>
       </c>
       <c r="C18" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>270</v>
       </c>
       <c r="B19" t="s">
-        <v>267</v>
+        <v>379</v>
       </c>
       <c r="C19" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>276</v>
       </c>
       <c r="B20" t="s">
-        <v>280</v>
+        <v>380</v>
       </c>
       <c r="C20" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>283</v>
       </c>
       <c r="B21" t="s">
-        <v>280</v>
+        <v>380</v>
       </c>
       <c r="C21" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>289</v>
       </c>
       <c r="B22" t="s">
-        <v>280</v>
+        <v>380</v>
       </c>
       <c r="C22" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>295</v>
       </c>
       <c r="B23" t="s">
-        <v>280</v>
+        <v>380</v>
       </c>
       <c r="C23" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>298</v>
       </c>
       <c r="B24" t="s">
-        <v>280</v>
+        <v>380</v>
       </c>
       <c r="C24" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>302</v>
       </c>
       <c r="B25" t="s">
-        <v>305</v>
+        <v>381</v>
       </c>
       <c r="C25" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>310</v>
       </c>
       <c r="B26" t="s">
-        <v>305</v>
+        <v>381</v>
       </c>
       <c r="C26" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>316</v>
       </c>
       <c r="B27" t="s">
-        <v>305</v>
+        <v>381</v>
       </c>
       <c r="C27" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>321</v>
       </c>
       <c r="B28" t="s">
-        <v>305</v>
+        <v>381</v>
       </c>
       <c r="C28" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>326</v>
       </c>
       <c r="B29" t="s">
-        <v>305</v>
+        <v>381</v>
       </c>
       <c r="C29" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>331</v>
       </c>
       <c r="B30" t="s">
-        <v>305</v>
+        <v>381</v>
       </c>
       <c r="C30" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>336</v>
       </c>
@@ -7523,8 +7628,11 @@
       <c r="C31" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>345</v>
       </c>
@@ -7534,19 +7642,25 @@
       <c r="C32" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>367</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C33" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>350</v>
       </c>
@@ -7556,8 +7670,11 @@
       <c r="C34" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>356</v>
       </c>
@@ -7567,8 +7684,11 @@
       <c r="C35" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>362</v>
       </c>
@@ -7578,16 +7698,22 @@
       <c r="C36" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>373</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>377</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>377</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
coded half of the data
</commit_message>
<xml_diff>
--- a/analysis/praise-draw_data.xlsx
+++ b/analysis/praise-draw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinkcupcakes123/Documents/Stanford/Social Learning Lab/GitHub/praise-draw/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25884A93-4A4C-8845-BE74-4AE80051F130}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5CFEEF-FF75-3443-97AC-F04B9BF4752C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" activeTab="2" xr2:uid="{7F85E784-ACEF-194A-84B2-6A49ADD88783}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3211" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3440" uniqueCount="657">
   <si>
     <t>count</t>
   </si>
@@ -1818,9 +1818,6 @@
     <t>cuz she wanted it to be perfect</t>
   </si>
   <si>
-    <t>practice_match</t>
-  </si>
-  <si>
     <t>PD4_191027_01</t>
   </si>
   <si>
@@ -1903,6 +1900,111 @@
   </si>
   <si>
     <t>nice I think? she does look nice</t>
+  </si>
+  <si>
+    <t>PD4_191110_01</t>
+  </si>
+  <si>
+    <t>time_out</t>
+  </si>
+  <si>
+    <t>hard_tracing</t>
+  </si>
+  <si>
+    <t>hard_tracing_explanation</t>
+  </si>
+  <si>
+    <t>selective_explanation</t>
+  </si>
+  <si>
+    <t>classroom_prefer</t>
+  </si>
+  <si>
+    <t>classroom_prefer_explanation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first kid with new format, everyone practices no forced choice; the second memcheck was kind of iffy, unfortunately you can't see it in the video but it looked like he almost said the right ones but kind of pointed to one of the bad ones, on the edge for including; was not chatty and wouldn't provide explanations for anything </t>
+  </si>
+  <si>
+    <t>PD4_191110_02</t>
+  </si>
+  <si>
+    <t>because it's in the lines</t>
+  </si>
+  <si>
+    <t>because…not sure</t>
+  </si>
+  <si>
+    <t>because he did it into the lines</t>
+  </si>
+  <si>
+    <t>because she thinks they're all good</t>
+  </si>
+  <si>
+    <t>because she…not sure</t>
+  </si>
+  <si>
+    <t>PD4_191110_03</t>
+  </si>
+  <si>
+    <t>because that [bad] is scribble and that one [good] is not it's tracing the lines</t>
+  </si>
+  <si>
+    <t>no (of letters)</t>
+  </si>
+  <si>
+    <t>because she put stars on every one</t>
+  </si>
+  <si>
+    <t>because she can help me</t>
+  </si>
+  <si>
+    <t>because they look like letters</t>
+  </si>
+  <si>
+    <t>because they are all good drawings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">because she can, if we’re doing tracings, she can tell me if it's good or not </t>
+  </si>
+  <si>
+    <t>PD4_191110_04</t>
+  </si>
+  <si>
+    <t>because she is all the good ones</t>
+  </si>
+  <si>
+    <t>because so these are the better ones and these are not traced</t>
+  </si>
+  <si>
+    <t>because those three are not good</t>
+  </si>
+  <si>
+    <t>maybe she liked all of them, or all of them were right</t>
+  </si>
+  <si>
+    <t>because she gave three stars and not to the bad ones</t>
+  </si>
+  <si>
+    <t>PD4_191110_05</t>
+  </si>
+  <si>
+    <t>because this one [bad] is like scribble scrabble and this one [good] is in the lines</t>
+  </si>
+  <si>
+    <t>because the scribble scrabble ones that he draw, she [linda] put a star and the ones that were good she [linda] also put a star so all of them were good but the ones that were scribble scrabble she [karen] said okay but the ones that were really good she [karen] will do the class</t>
+  </si>
+  <si>
+    <t>because she [karen] did the good drawings but she [linda] did it in the good and bad drawings but she [karen] did it only in the good drawings which is the better one</t>
+  </si>
+  <si>
+    <t>because they look good and he wrote it right in the lines</t>
+  </si>
+  <si>
+    <t>because she thinks, she's just like nice but this one is not good and this one is not good and this one is not good</t>
+  </si>
+  <si>
+    <t>because she told better</t>
   </si>
 </sst>
 </file>
@@ -1925,12 +2027,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1945,11 +2053,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11790,10 +11899,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F37BCAE-525E-6748-9017-84BC60860672}">
-  <dimension ref="A1:AE14"/>
+  <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11819,15 +11928,21 @@
     <col min="20" max="20" width="18.1640625" customWidth="1"/>
     <col min="21" max="21" width="15.83203125" customWidth="1"/>
     <col min="22" max="22" width="19.33203125" customWidth="1"/>
-    <col min="23" max="25" width="14.5" customWidth="1"/>
+    <col min="23" max="24" width="14.5" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" customWidth="1"/>
     <col min="26" max="26" width="15.5" customWidth="1"/>
     <col min="27" max="27" width="18" customWidth="1"/>
     <col min="28" max="28" width="11.5" customWidth="1"/>
     <col min="29" max="29" width="20.1640625" customWidth="1"/>
-    <col min="30" max="30" width="20.33203125" customWidth="1"/>
+    <col min="30" max="30" width="11.83203125" customWidth="1"/>
+    <col min="31" max="31" width="22.1640625" customWidth="1"/>
+    <col min="32" max="32" width="19.83203125" customWidth="1"/>
+    <col min="33" max="33" width="20.33203125" customWidth="1"/>
+    <col min="34" max="34" width="16.83203125" customWidth="1"/>
+    <col min="35" max="35" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11901,7 +12016,7 @@
         <v>550</v>
       </c>
       <c r="Y1" t="s">
-        <v>594</v>
+        <v>623</v>
       </c>
       <c r="Z1" t="s">
         <v>559</v>
@@ -11916,13 +12031,28 @@
         <v>407</v>
       </c>
       <c r="AD1" t="s">
+        <v>624</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>625</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>626</v>
+      </c>
+      <c r="AG1" t="s">
         <v>553</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
+        <v>627</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>628</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11995,8 +12125,8 @@
       <c r="X2" t="s">
         <v>46</v>
       </c>
-      <c r="Y2">
-        <v>0</v>
+      <c r="Y2" t="s">
+        <v>68</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -12011,13 +12141,28 @@
         <v>68</v>
       </c>
       <c r="AD2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG2" t="s">
         <v>554</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AH2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12090,8 +12235,8 @@
       <c r="X3" t="s">
         <v>46</v>
       </c>
-      <c r="Y3">
-        <v>0</v>
+      <c r="Y3" t="s">
+        <v>68</v>
       </c>
       <c r="Z3">
         <v>0</v>
@@ -12106,13 +12251,28 @@
         <v>244</v>
       </c>
       <c r="AD3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG3" t="s">
         <v>561</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AH3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ3" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12185,8 +12345,8 @@
       <c r="X4" t="s">
         <v>42</v>
       </c>
-      <c r="Y4">
-        <v>1</v>
+      <c r="Y4" t="s">
+        <v>68</v>
       </c>
       <c r="Z4">
         <v>10</v>
@@ -12201,13 +12361,28 @@
         <v>567</v>
       </c>
       <c r="AD4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG4" t="s">
         <v>568</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AH4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12280,8 +12455,8 @@
       <c r="X5" t="s">
         <v>42</v>
       </c>
-      <c r="Y5">
-        <v>0</v>
+      <c r="Y5" t="s">
+        <v>68</v>
       </c>
       <c r="Z5">
         <v>7</v>
@@ -12296,13 +12471,28 @@
         <v>572</v>
       </c>
       <c r="AD5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG5" t="s">
         <v>574</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AH5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -12375,8 +12565,8 @@
       <c r="X6" t="s">
         <v>46</v>
       </c>
-      <c r="Y6">
-        <v>1</v>
+      <c r="Y6" t="s">
+        <v>68</v>
       </c>
       <c r="Z6">
         <v>0</v>
@@ -12391,13 +12581,28 @@
         <v>577</v>
       </c>
       <c r="AD6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG6" t="s">
         <v>244</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AH6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -12470,8 +12675,8 @@
       <c r="X7" t="s">
         <v>46</v>
       </c>
-      <c r="Y7">
-        <v>0</v>
+      <c r="Y7" t="s">
+        <v>68</v>
       </c>
       <c r="Z7">
         <v>0</v>
@@ -12486,10 +12691,25 @@
         <v>581</v>
       </c>
       <c r="AD7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG7" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -12562,8 +12782,8 @@
       <c r="X8" t="s">
         <v>46</v>
       </c>
-      <c r="Y8">
-        <v>1</v>
+      <c r="Y8" t="s">
+        <v>68</v>
       </c>
       <c r="Z8">
         <v>0</v>
@@ -12578,10 +12798,25 @@
         <v>586</v>
       </c>
       <c r="AD8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG8" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12654,8 +12889,8 @@
       <c r="X9" t="s">
         <v>42</v>
       </c>
-      <c r="Y9">
-        <v>1</v>
+      <c r="Y9" t="s">
+        <v>68</v>
       </c>
       <c r="Z9">
         <v>9</v>
@@ -12670,15 +12905,30 @@
         <v>592</v>
       </c>
       <c r="AD9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG9" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C10" s="2">
         <v>43765</v>
@@ -12708,7 +12958,7 @@
         <v>67</v>
       </c>
       <c r="L10" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="M10" t="s">
         <v>43</v>
@@ -12746,34 +12996,49 @@
       <c r="X10" t="s">
         <v>46</v>
       </c>
-      <c r="Y10">
-        <v>0</v>
+      <c r="Y10" t="s">
+        <v>68</v>
       </c>
       <c r="Z10">
         <v>0</v>
       </c>
       <c r="AA10" t="s">
+        <v>600</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>602</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>603</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ10" t="s">
         <v>601</v>
       </c>
-      <c r="AB10" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>603</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>604</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C11" s="2">
         <v>43765</v>
@@ -12803,7 +13068,7 @@
         <v>67</v>
       </c>
       <c r="L11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="M11" t="s">
         <v>77</v>
@@ -12841,34 +13106,49 @@
       <c r="X11" t="s">
         <v>42</v>
       </c>
-      <c r="Y11">
-        <v>0</v>
+      <c r="Y11" t="s">
+        <v>68</v>
       </c>
       <c r="Z11">
         <v>12</v>
       </c>
       <c r="AA11" t="s">
+        <v>606</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC11" t="s">
         <v>607</v>
       </c>
-      <c r="AB11" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG11" t="s">
         <v>608</v>
       </c>
-      <c r="AD11" t="s">
-        <v>609</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C12" s="2">
         <v>43765</v>
@@ -12898,7 +13178,7 @@
         <v>67</v>
       </c>
       <c r="L12" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="M12" t="s">
         <v>77</v>
@@ -12936,34 +13216,49 @@
       <c r="X12" t="s">
         <v>42</v>
       </c>
-      <c r="Y12">
-        <v>0</v>
+      <c r="Y12" t="s">
+        <v>68</v>
       </c>
       <c r="Z12">
         <v>7</v>
       </c>
       <c r="AA12" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC12" t="s">
         <v>612</v>
       </c>
-      <c r="AB12" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG12" t="s">
         <v>613</v>
       </c>
-      <c r="AD12" t="s">
-        <v>614</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C13" s="2">
         <v>43765</v>
@@ -12993,7 +13288,7 @@
         <v>67</v>
       </c>
       <c r="L13" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="M13" t="s">
         <v>43</v>
@@ -13031,31 +13326,46 @@
       <c r="X13" t="s">
         <v>46</v>
       </c>
-      <c r="Y13">
-        <v>0</v>
+      <c r="Y13" t="s">
+        <v>68</v>
       </c>
       <c r="Z13">
         <v>0</v>
       </c>
       <c r="AA13" t="s">
+        <v>615</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC13" t="s">
         <v>616</v>
       </c>
-      <c r="AB13" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG13" t="s">
         <v>617</v>
       </c>
-      <c r="AD13" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C14" s="2">
         <v>43765</v>
@@ -13085,7 +13395,7 @@
         <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="M14" t="s">
         <v>43</v>
@@ -13123,23 +13433,536 @@
       <c r="X14" t="s">
         <v>42</v>
       </c>
-      <c r="Y14">
-        <v>1</v>
+      <c r="Y14" t="s">
+        <v>68</v>
       </c>
       <c r="Z14">
         <v>6</v>
       </c>
       <c r="AA14" t="s">
+        <v>619</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC14" t="s">
         <v>620</v>
       </c>
-      <c r="AB14" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG14" t="s">
         <v>621</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AH14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>622</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43779</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>429</v>
+      </c>
+      <c r="I15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" t="s">
+        <v>401</v>
+      </c>
+      <c r="M15" t="s">
+        <v>43</v>
+      </c>
+      <c r="N15" t="s">
+        <v>44</v>
+      </c>
+      <c r="O15" t="s">
+        <v>44</v>
+      </c>
+      <c r="P15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>77</v>
+      </c>
+      <c r="R15" t="s">
+        <v>42</v>
+      </c>
+      <c r="S15" t="s">
+        <v>77</v>
+      </c>
+      <c r="T15" t="s">
+        <v>43</v>
+      </c>
+      <c r="U15" t="s">
+        <v>46</v>
+      </c>
+      <c r="V15" t="s">
+        <v>68</v>
+      </c>
+      <c r="W15" t="s">
+        <v>44</v>
+      </c>
+      <c r="X15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z15" s="4"/>
+      <c r="AA15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>401</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>401</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>401</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>401</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>630</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43779</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" t="s">
+        <v>429</v>
+      </c>
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" t="s">
+        <v>631</v>
+      </c>
+      <c r="M16" t="s">
+        <v>43</v>
+      </c>
+      <c r="N16" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" t="s">
+        <v>44</v>
+      </c>
+      <c r="P16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>43</v>
+      </c>
+      <c r="R16" t="s">
+        <v>46</v>
+      </c>
+      <c r="S16" t="s">
+        <v>68</v>
+      </c>
+      <c r="T16" t="s">
+        <v>43</v>
+      </c>
+      <c r="U16" t="s">
+        <v>46</v>
+      </c>
+      <c r="V16" t="s">
+        <v>68</v>
+      </c>
+      <c r="W16" t="s">
+        <v>45</v>
+      </c>
+      <c r="X16" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z16" s="4"/>
+      <c r="AA16" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>632</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>632</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>633</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>634</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>636</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43779</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" t="s">
+        <v>429</v>
+      </c>
+      <c r="I17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" t="s">
+        <v>637</v>
+      </c>
+      <c r="M17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" t="s">
+        <v>45</v>
+      </c>
+      <c r="P17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>43</v>
+      </c>
+      <c r="R17" t="s">
+        <v>46</v>
+      </c>
+      <c r="S17" t="s">
+        <v>68</v>
+      </c>
+      <c r="T17" t="s">
+        <v>43</v>
+      </c>
+      <c r="U17" t="s">
+        <v>46</v>
+      </c>
+      <c r="V17" t="s">
+        <v>68</v>
+      </c>
+      <c r="W17" t="s">
+        <v>44</v>
+      </c>
+      <c r="X17" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>638</v>
+      </c>
+      <c r="Z17" s="4"/>
+      <c r="AA17" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>639</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>640</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>641</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>642</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>644</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43779</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" t="s">
+        <v>429</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" t="s">
+        <v>590</v>
+      </c>
+      <c r="L18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" t="s">
+        <v>43</v>
+      </c>
+      <c r="N18" t="s">
+        <v>44</v>
+      </c>
+      <c r="O18" t="s">
+        <v>45</v>
+      </c>
+      <c r="P18" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" t="s">
+        <v>46</v>
+      </c>
+      <c r="S18" t="s">
+        <v>68</v>
+      </c>
+      <c r="T18" t="s">
+        <v>43</v>
+      </c>
+      <c r="U18" t="s">
+        <v>46</v>
+      </c>
+      <c r="V18" t="s">
+        <v>68</v>
+      </c>
+      <c r="W18" t="s">
+        <v>45</v>
+      </c>
+      <c r="X18" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z18" s="4"/>
+      <c r="AA18" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>645</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>646</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>647</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>648</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>650</v>
+      </c>
+      <c r="C19" s="2">
+        <v>43779</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" t="s">
+        <v>429</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" t="s">
+        <v>651</v>
+      </c>
+      <c r="M19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P19" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>43</v>
+      </c>
+      <c r="R19" t="s">
+        <v>46</v>
+      </c>
+      <c r="S19" t="s">
+        <v>68</v>
+      </c>
+      <c r="T19" t="s">
+        <v>43</v>
+      </c>
+      <c r="U19" t="s">
+        <v>46</v>
+      </c>
+      <c r="V19" t="s">
+        <v>68</v>
+      </c>
+      <c r="W19" t="s">
+        <v>44</v>
+      </c>
+      <c r="X19" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z19" s="4"/>
+      <c r="AA19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>652</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>653</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>654</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>655</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added column for which version
</commit_message>
<xml_diff>
--- a/analysis/praise-draw_data.xlsx
+++ b/analysis/praise-draw_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinkcupcakes123/Documents/Stanford/Social Learning Lab/GitHub/praise-draw/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masaba/Documents/GitHub/praise-draw/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CC2F1B-2CD8-4B47-A6CC-1791ADF9044E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB65A4F-C6EF-0D41-8141-703EC6897936}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" activeTab="2" xr2:uid="{7F85E784-ACEF-194A-84B2-6A49ADD88783}"/>
+    <workbookView xWindow="-38100" yWindow="-900" windowWidth="37320" windowHeight="21140" activeTab="2" xr2:uid="{7F85E784-ACEF-194A-84B2-6A49ADD88783}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilot 1" sheetId="1" r:id="rId1"/>
@@ -18,23 +18,20 @@
     <sheet name="Pilot 4" sheetId="5" r:id="rId3"/>
     <sheet name="Quality Ratings" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Pilot 4'!$A$1:$AK$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3445" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="658">
   <si>
     <t>count</t>
   </si>
@@ -2005,6 +2002,9 @@
   </si>
   <si>
     <t>because she told better</t>
+  </si>
+  <si>
+    <t>forced_choice_version</t>
   </si>
 </sst>
 </file>
@@ -11894,10 +11894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F37BCAE-525E-6748-9017-84BC60860672}">
-  <dimension ref="A1:AJ19"/>
+  <dimension ref="A1:AK19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ19" sqref="AJ19"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11925,7 +11925,7 @@
     <col min="22" max="22" width="19.33203125" customWidth="1"/>
     <col min="23" max="24" width="14.5" customWidth="1"/>
     <col min="25" max="25" width="12.83203125" customWidth="1"/>
-    <col min="26" max="26" width="15.5" customWidth="1"/>
+    <col min="26" max="26" width="21.1640625" customWidth="1"/>
     <col min="27" max="27" width="18" customWidth="1"/>
     <col min="28" max="28" width="11.5" customWidth="1"/>
     <col min="29" max="29" width="20.1640625" customWidth="1"/>
@@ -11934,10 +11934,10 @@
     <col min="32" max="32" width="19.83203125" customWidth="1"/>
     <col min="33" max="33" width="20.33203125" customWidth="1"/>
     <col min="34" max="34" width="16.83203125" customWidth="1"/>
-    <col min="35" max="35" width="25.6640625" customWidth="1"/>
+    <col min="35" max="36" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12044,10 +12044,13 @@
         <v>628</v>
       </c>
       <c r="AJ1" t="s">
+        <v>657</v>
+      </c>
+      <c r="AK1" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12153,11 +12156,14 @@
       <c r="AI2" t="s">
         <v>68</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AJ2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK2" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12263,11 +12269,14 @@
       <c r="AI3" t="s">
         <v>68</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AJ3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK3" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12373,11 +12382,14 @@
       <c r="AI4" t="s">
         <v>68</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AJ4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK4" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12483,11 +12495,14 @@
       <c r="AI5" t="s">
         <v>68</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AJ5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK5" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -12593,11 +12608,14 @@
       <c r="AI6" t="s">
         <v>68</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AJ6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK6" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -12703,8 +12721,11 @@
       <c r="AI7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AJ7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -12810,8 +12831,11 @@
       <c r="AI8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AJ8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12917,8 +12941,11 @@
       <c r="AI9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AJ9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -13024,11 +13051,14 @@
       <c r="AI10" t="s">
         <v>68</v>
       </c>
-      <c r="AJ10" t="s">
+      <c r="AJ10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK10" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -13134,11 +13164,14 @@
       <c r="AI11" t="s">
         <v>68</v>
       </c>
-      <c r="AJ11" t="s">
+      <c r="AJ11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK11" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -13244,11 +13277,14 @@
       <c r="AI12" t="s">
         <v>68</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AJ12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK12" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -13354,8 +13390,11 @@
       <c r="AI13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AJ13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -13461,8 +13500,11 @@
       <c r="AI14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AJ14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -13568,11 +13610,14 @@
       <c r="AI15" t="s">
         <v>401</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AJ15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK15" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -13678,8 +13723,11 @@
       <c r="AI16" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -13785,8 +13833,11 @@
       <c r="AI17" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -13892,8 +13943,11 @@
       <c r="AI18" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -13999,8 +14053,12 @@
       <c r="AI19" t="s">
         <v>656</v>
       </c>
+      <c r="AJ19" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AK19" xr:uid="{6C8AC2CA-7D33-6D49-B0D9-F717B4229F4D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>